<commit_message>
spam y boome_equipo rojo
</commit_message>
<xml_diff>
--- a/Adivina Quien.xlsx
+++ b/Adivina Quien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Documents\Svhool\ITSJR\9no Semestre\Inteligencia Artificial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorio_IA\IA2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE90D9E-C7B2-4FB5-BF41-D9C9532E35D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FE63B9-A765-43F1-875A-4121A6249810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8BE19EE0-0C00-42A2-AE05-B2EFB1EC2168}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8BE19EE0-0C00-42A2-AE05-B2EFB1EC2168}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -214,9 +214,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -224,6 +221,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -244,7 +244,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -543,66 +543,66 @@
   <dimension ref="B1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>512</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>256</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>128</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>64</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>32</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>16</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>8</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>4</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>2</v>
       </c>
-      <c r="L2" s="5">
-        <v>1</v>
-      </c>
-      <c r="M2" s="5" t="s">
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -842,7 +842,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>544</v>
       </c>
     </row>
@@ -877,62 +877,62 @@
       <c r="K13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="8"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>512</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>256</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>128</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>64</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>32</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <v>16</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="4">
         <v>8</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="4">
         <v>4</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="4">
         <v>2</v>
       </c>
-      <c r="L16" s="5">
-        <v>1</v>
-      </c>
-      <c r="M16" s="5" t="s">
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
       <c r="L26" s="3">
         <v>1</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26" s="6">
         <v>5</v>
       </c>
     </row>
@@ -1207,10 +1207,10 @@
       <c r="K27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L27" s="6" t="s">
+      <c r="L27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="8"/>
+      <c r="M27" s="7"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>

</xml_diff>